<commit_message>
editing integration testing sheet , names of modules were not accurate
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/integrationnTestCases.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/integrationnTestCases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="71">
   <si>
     <t>objective</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t xml:space="preserve"> LCD will clear the screens</t>
-  </si>
-  <si>
-    <t>timer vs. DIO</t>
   </si>
   <si>
     <t>to test the timer module with DIO PINS related to the timer.</t>
@@ -322,13 +319,6 @@
     <t>To test the integration between all system modules</t>
   </si>
   <si>
-    <t xml:space="preserve">LCD
-Switch
-Timer
-DIO
-</t>
-  </si>
-  <si>
     <t>Atmega32 microcontroller
 LCD 16X2 module</t>
   </si>
@@ -408,9 +398,6 @@
     <t>Project Name</t>
   </si>
   <si>
-    <t>Reference Document</t>
-  </si>
-  <si>
     <t>Created by</t>
   </si>
   <si>
@@ -513,7 +500,10 @@
     <t>LCD -DIO module</t>
   </si>
   <si>
-    <t>LCD - Switch module</t>
+    <t>timer - DIO mdules</t>
+  </si>
+  <si>
+    <t>LCD - Switch modules</t>
   </si>
 </sst>
 </file>
@@ -672,7 +662,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
@@ -712,35 +702,38 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1043,10 +1036,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I25"/>
+  <dimension ref="A2:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1079,10 +1072,10 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="5"/>
@@ -1093,9 +1086,11 @@
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -1105,10 +1100,10 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="D5" s="13">
+        <v>42525</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="5"/>
@@ -1119,10 +1114,10 @@
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" s="13">
-        <v>42525</v>
+        <v>42586</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="5"/>
@@ -1132,267 +1127,272 @@
     <row r="7" spans="1:9">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" s="6" customFormat="1" ht="30">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="124.9" customHeight="1">
+      <c r="A9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="13">
-        <v>42586</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" ht="30">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="124.9" customHeight="1">
-      <c r="A10" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="23" t="s">
+      <c r="I9" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="70.900000000000006" customHeight="1">
+      <c r="A10" s="24"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="79.150000000000006" customHeight="1">
+      <c r="A11" s="24"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="8" customFormat="1">
+      <c r="I12" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="79.900000000000006" customHeight="1">
+      <c r="A13" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="64.150000000000006" customHeight="1">
+      <c r="A14" s="24"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="78.599999999999994" customHeight="1">
+      <c r="A15" s="24"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="8" customFormat="1">
+      <c r="I16" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="90">
+      <c r="A17" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="8" customFormat="1">
+      <c r="A18" s="17"/>
+      <c r="I18" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="74.45" customHeight="1">
+      <c r="A19" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="70.900000000000006" customHeight="1">
-      <c r="A11" s="20"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="79.150000000000006" customHeight="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="8" customFormat="1">
-      <c r="I13" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="79.900000000000006" customHeight="1">
-      <c r="A14" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="64.150000000000006" customHeight="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="78.599999999999994" customHeight="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="7" t="s">
+      <c r="C19" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="I19" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="88.15" customHeight="1">
+      <c r="A20" s="24"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I16" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="8" customFormat="1">
-      <c r="I17" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="90">
-      <c r="A18" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="8" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="I19" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="74.45" customHeight="1">
-      <c r="A20" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="88.15" customHeight="1">
-      <c r="A21" s="20"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
+      <c r="I20" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="73.900000000000006" customHeight="1">
+      <c r="A21" s="24"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="20"/>
       <c r="F21" s="7" t="s">
         <v>42</v>
       </c>
@@ -1400,86 +1400,72 @@
         <v>43</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I21" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="I21" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="73.900000000000006" customHeight="1">
-      <c r="A22" s="20"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="7" t="s">
+    </row>
+    <row r="22" spans="1:9" s="8" customFormat="1">
+      <c r="I22" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="137.44999999999999" customHeight="1">
+      <c r="A23" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="19" t="e">
+        <f>-LCD
+-Switch
+-Timer
+-DIO
+                                                                                                                                                                                                                                                                modules</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="F23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="8" customFormat="1">
-      <c r="I23" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="137.44999999999999" customHeight="1">
-      <c r="A24" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I24" s="19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="8" customFormat="1"/>
+      <c r="H23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="8" customFormat="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" display="© www.SoftwareTestingHelp.com Team"/>
+    <hyperlink ref="D8" r:id="rId1" display="© www.SoftwareTestingHelp.com Team"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>